<commit_message>
Implement logic to display product list and search funtions in restorck form
</commit_message>
<xml_diff>
--- a/documentation/Version History.xlsx
+++ b/documentation/Version History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\MiniMarketInventoryManagement\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E627CC5F-2E44-4793-B31E-FE52F7FE4548}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBAC42C-F00D-472C-95D0-FE0C934E9B6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7D18C05-31F1-4F48-87A8-61387A74A440}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t xml:space="preserve">Mechanics </t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>Returns Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intermediate Product Management </t>
+  </si>
+  <si>
+    <t>Restock Product Form</t>
   </si>
 </sst>
 </file>
@@ -315,58 +321,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -688,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3F8C43-F028-4E57-9D96-908845B50375}">
   <dimension ref="A2:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G20"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,297 +706,297 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="19">
+      <c r="F5" s="4"/>
+      <c r="G5" s="11">
         <v>43853</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="19">
         <v>43856</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="14" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="16" t="s">
+      <c r="D8" s="16"/>
+      <c r="E8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="19">
         <v>43859</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="15" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="15" t="s">
+      <c r="D9" s="17"/>
+      <c r="E9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="14" t="s">
+      <c r="A10" s="14"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="17" t="s">
+      <c r="D10" s="21"/>
+      <c r="E10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="19">
         <v>43862</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="15" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="15" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="18"/>
+      <c r="E13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="18" t="s">
         <v>55</v>
       </c>
       <c r="G13" s="22"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="14" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="21"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="7" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="19">
         <v>43872</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="17" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="21"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="16"/>
+      <c r="C17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="19">
         <v>43875</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="18" t="s">
+      <c r="D18" s="17"/>
+      <c r="E18" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="10"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="22"/>
     </row>
     <row r="19" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="18" t="s">
+      <c r="A19" s="14"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G19" s="22"/>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="14" t="s">
+      <c r="A20" s="14"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="14" t="s">
+      <c r="D20" s="21"/>
+      <c r="E20" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="21"/>
+      <c r="G20" s="20"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -1046,36 +1052,36 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -1101,9 +1107,13 @@
       <c r="B30" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="E30" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="F30" s="2" t="s">
         <v>49</v>
       </c>
@@ -1248,38 +1258,6 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="G17:G20"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="G6:G7"/>
@@ -1293,6 +1271,38 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G20"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D17:D20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finish Foundational FIFO/LIFO inventory management system with returns, restock, and voiding transactions
</commit_message>
<xml_diff>
--- a/documentation/Version History.xlsx
+++ b/documentation/Version History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\MiniMarketInventoryManagement\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C9502D-F72C-44FE-920B-055B6538EF31}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39EEEDE-3BCD-40BA-944D-8C6AC8135C0A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7D18C05-31F1-4F48-87A8-61387A74A440}"/>
   </bookViews>
@@ -246,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -306,11 +306,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -318,9 +398,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -376,6 +453,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -694,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3F8C43-F028-4E57-9D96-908845B50375}">
   <dimension ref="A2:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,297 +810,297 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="11">
+      <c r="F5" s="3"/>
+      <c r="G5" s="10">
         <v>43853</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="18">
         <v>43856</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="6" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="8" t="s">
+      <c r="D8" s="15"/>
+      <c r="E8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="18">
         <v>43859</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="7" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="16"/>
+      <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="22"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="6" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="9" t="s">
+      <c r="D10" s="20"/>
+      <c r="E10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="18">
         <v>43862</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="7" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="22"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="21"/>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="7" t="s">
+      <c r="A13" s="13"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="17" t="s">
+      <c r="D13" s="17"/>
+      <c r="E13" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="22"/>
+      <c r="G13" s="21"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="6" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="20"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="12" t="s">
+      <c r="D15" s="15"/>
+      <c r="E15" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="18">
         <v>43872</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="9" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="20"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="15"/>
+      <c r="C17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="18">
         <v>43875</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17" t="s">
+      <c r="A18" s="13"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="10" t="s">
+      <c r="D18" s="16"/>
+      <c r="E18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="22"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="21"/>
     </row>
     <row r="19" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="10" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="22"/>
+      <c r="G19" s="21"/>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="6" t="s">
+      <c r="A20" s="13"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="6" t="s">
+      <c r="D20" s="20"/>
+      <c r="E20" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="20"/>
+      <c r="G20" s="19"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -1052,83 +1156,85 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="3" t="s">
+      <c r="D29" s="15"/>
+      <c r="E29" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="3" t="s">
+      <c r="G29" s="24">
+        <v>43882</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="3" t="s">
+      <c r="D30" s="16"/>
+      <c r="E30" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="2"/>
+      <c r="G30" s="27"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2" t="s">
+      <c r="A31" s="28"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G31" s="2"/>
+      <c r="G31" s="30"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
@@ -1257,7 +1363,13 @@
       <c r="G45" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="51">
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B30:B31"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="G6:G7"/>

</xml_diff>

<commit_message>
Refactor code to include namespaces
</commit_message>
<xml_diff>
--- a/documentation/Version History.xlsx
+++ b/documentation/Version History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\MiniMarketInventoryManagement\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39EEEDE-3BCD-40BA-944D-8C6AC8135C0A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8692A344-7B9C-413E-9DD8-0D31B0BF050C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7D18C05-31F1-4F48-87A8-61387A74A440}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t xml:space="preserve">Mechanics </t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>Restock Product Form</t>
+  </si>
+  <si>
+    <t>Code Refactoring (Namespaces)</t>
+  </si>
+  <si>
+    <t>v0.6.1</t>
   </si>
 </sst>
 </file>
@@ -246,7 +252,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -386,11 +392,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -422,64 +465,76 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -799,7 +854,7 @@
   <dimension ref="A2:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,36 +865,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -870,237 +925,237 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="30" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="28">
         <v>43856</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="19"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="15"/>
+      <c r="D8" s="21"/>
       <c r="E8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="28">
         <v>43859</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="16"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="16"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="21"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="31"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="20"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="19"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="29"/>
     </row>
     <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="30" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="28">
         <v>43862</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="17"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="21"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="17"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="16" t="s">
+      <c r="D13" s="24"/>
+      <c r="E13" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="21"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="19"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="29"/>
     </row>
     <row r="15" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="11" t="s">
+      <c r="D15" s="21"/>
+      <c r="E15" s="30" t="s">
         <v>36</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="28">
         <v>43872</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="12"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="25"/>
       <c r="F16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="19"/>
+      <c r="G16" s="29"/>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="15"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="21" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="28">
         <v>43875</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16" t="s">
+      <c r="A18" s="27"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="21"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="31"/>
     </row>
     <row r="19" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="9" t="s">
         <v>46</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="21"/>
+      <c r="G19" s="31"/>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="20"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="20"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="19"/>
+      <c r="G20" s="29"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -1156,94 +1211,98 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="13" t="s">
         <v>50</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="23" t="s">
+      <c r="D29" s="21"/>
+      <c r="E29" s="12" t="s">
         <v>57</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="16">
         <v>43882</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="17" t="s">
+      <c r="A30" s="14"/>
+      <c r="B30" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="26" t="s">
+      <c r="D30" s="22"/>
+      <c r="E30" s="19" t="s">
         <v>59</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="27"/>
+      <c r="G30" s="17"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="29"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="20"/>
       <c r="F31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G31" s="30"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="A32" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="34"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
@@ -1363,44 +1422,8 @@
       <c r="G45" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G20"/>
+  <mergeCells count="52">
+    <mergeCell ref="B32:G32"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="A15:A16"/>
@@ -1415,6 +1438,43 @@
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D17:D20"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G20"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B30:B31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Establish major refactoring of businesslayer
</commit_message>
<xml_diff>
--- a/documentation/Version History.xlsx
+++ b/documentation/Version History.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\MiniMarketInventoryManagement\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siclait\Desktop\MiniMarketInventoryManagement\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8692A344-7B9C-413E-9DD8-0D31B0BF050C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4FD042-2FD5-4328-B40B-D8B2315BBB70}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7D18C05-31F1-4F48-87A8-61387A74A440}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{F7D18C05-31F1-4F48-87A8-61387A74A440}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
   <si>
     <t xml:space="preserve">Mechanics </t>
   </si>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>v0.6.1</t>
+  </si>
+  <si>
+    <t>21 Fed</t>
+  </si>
+  <si>
+    <t>v0.6.2</t>
+  </si>
+  <si>
+    <t>22 Fed</t>
+  </si>
+  <si>
+    <t>Code Refactoring (Business Layer Namespaces)</t>
   </si>
 </sst>
 </file>
@@ -433,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -471,6 +483,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -495,47 +552,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,7 +573,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -854,10 +872,10 @@
   <dimension ref="A2:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
@@ -865,36 +883,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -925,10 +943,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -937,29 +955,29 @@
       <c r="D6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="25">
         <v>43856</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="29"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="26"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="21"/>
@@ -973,47 +991,47 @@
       <c r="F8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="25">
         <v>43859</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="22"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="31"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="23"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="29"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="17" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="21" t="s">
@@ -1022,81 +1040,81 @@
       <c r="F11" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="25">
         <v>43862</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="24"/>
       <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="24"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="31"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="24"/>
       <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="24"/>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="23" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="31"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="29"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="21"/>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G15" s="25">
         <v>43872</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="25"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="29"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="19" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="21"/>
@@ -1112,50 +1130,50 @@
       <c r="F17" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="28">
+      <c r="G17" s="25">
         <v>43875</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="22"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="31"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="9" t="s">
         <v>46</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="31"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="23"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="23"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="29"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -1211,39 +1229,39 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="26" t="s">
+      <c r="F27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G27" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="28" t="s">
         <v>50</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1259,59 +1277,67 @@
       <c r="F29" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="16">
+      <c r="G29" s="31">
         <v>43882</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="19" t="s">
+      <c r="D30" s="23"/>
+      <c r="E30" s="34" t="s">
         <v>59</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="17"/>
+      <c r="G30" s="32"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="20"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="35"/>
       <c r="F31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G31" s="18"/>
+      <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="34"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="36" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="A33" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="36" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
@@ -1422,8 +1448,45 @@
       <c r="G45" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="B32:G32"/>
+  <mergeCells count="53">
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G20"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="A15:A16"/>
@@ -1439,45 +1502,9 @@
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D17:D20"/>
     <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G20"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B30:B31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemente keyboard shortcuts to inventory browser in tandem with the menubar
</commit_message>
<xml_diff>
--- a/documentation/Version History.xlsx
+++ b/documentation/Version History.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siclait\Desktop\MiniMarketInventoryManagement\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\MiniMarketInventoryManagement\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4FD042-2FD5-4328-B40B-D8B2315BBB70}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D601674-D020-48D0-BDA9-0FC3A38115BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{F7D18C05-31F1-4F48-87A8-61387A74A440}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7D18C05-31F1-4F48-87A8-61387A74A440}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t xml:space="preserve">Mechanics </t>
   </si>
@@ -229,6 +229,18 @@
   </si>
   <si>
     <t>Code Refactoring (Business Layer Namespaces)</t>
+  </si>
+  <si>
+    <t>v0.7.0</t>
+  </si>
+  <si>
+    <t>Menu Bar Shortcuts</t>
+  </si>
+  <si>
+    <t>Basic Report Analytics</t>
+  </si>
+  <si>
+    <t>Report Views</t>
   </si>
 </sst>
 </file>
@@ -445,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -486,6 +498,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -493,67 +508,67 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -573,7 +588,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -872,10 +887,10 @@
   <dimension ref="A2:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
@@ -883,36 +898,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="31" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -943,237 +958,237 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="35" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="33">
         <v>43856</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="26"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="21"/>
+      <c r="D8" s="26"/>
       <c r="E8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="33">
         <v>43859</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="36"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="22"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="26"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="34"/>
     </row>
     <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="35" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="33">
         <v>43862</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="24"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="27"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="24"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="23" t="s">
+      <c r="D13" s="29"/>
+      <c r="E13" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="27"/>
+      <c r="G13" s="36"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="26"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="34"/>
     </row>
     <row r="15" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="17" t="s">
+      <c r="D15" s="26"/>
+      <c r="E15" s="35" t="s">
         <v>36</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="33">
         <v>43872</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="18"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="30"/>
       <c r="F16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="26"/>
+      <c r="G16" s="34"/>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="21"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="26" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="33">
         <v>43875</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23" t="s">
+      <c r="A18" s="32"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="23"/>
+      <c r="D18" s="27"/>
       <c r="E18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="36"/>
     </row>
     <row r="19" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
       <c r="E19" s="9" t="s">
         <v>46</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="27"/>
+      <c r="G19" s="36"/>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="22"/>
+      <c r="D20" s="28"/>
       <c r="E20" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="26"/>
+      <c r="G20" s="34"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -1229,39 +1244,39 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="31" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="18" t="s">
         <v>50</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1270,57 +1285,57 @@
       <c r="C29" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="21"/>
+      <c r="D29" s="26"/>
       <c r="E29" s="12" t="s">
         <v>57</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="31">
+      <c r="G29" s="21">
         <v>43882</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="24" t="s">
+      <c r="A30" s="19"/>
+      <c r="B30" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="34" t="s">
+      <c r="D30" s="27"/>
+      <c r="E30" s="24" t="s">
         <v>59</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="32"/>
+      <c r="G30" s="22"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="35"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="25"/>
       <c r="F31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G31" s="33"/>
+      <c r="G31" s="23"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="36" t="s">
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="14" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1328,24 +1343,34 @@
       <c r="A33" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="36" t="s">
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="C34" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1449,44 +1474,6 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G20"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="A15:A16"/>
@@ -1501,7 +1488,45 @@
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D17:D20"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G20"/>
     <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B30:B31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
BUG FIX: implement child disposal logic in user registry form to close any opened user information template form
</commit_message>
<xml_diff>
--- a/documentation/Version History.xlsx
+++ b/documentation/Version History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\MiniMarketInventoryManagement\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B9CB59-CADE-461D-ADB5-DC31AA228F55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D420AE97-6993-4EE1-9388-17915ACF2983}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7D18C05-31F1-4F48-87A8-61387A74A440}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
   <si>
     <t xml:space="preserve">Mechanics </t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>B3</t>
+  </si>
+  <si>
+    <t>B2 = FIXED</t>
   </si>
 </sst>
 </file>
@@ -525,71 +528,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -908,7 +911,7 @@
   <dimension ref="A2:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,36 +922,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -979,263 +982,263 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="41" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="39">
         <v>43856</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="30"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="40"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="32"/>
       <c r="E8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="39">
         <v>43859</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="27"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="27"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="31"/>
+      <c r="G9" s="42"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="26"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="30"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="40"/>
     </row>
     <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="41" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="32" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="39">
         <v>43862</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="27"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="31"/>
+      <c r="G12" s="42"/>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="27" t="s">
+      <c r="D13" s="35"/>
+      <c r="E13" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="31"/>
+      <c r="G13" s="42"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="30"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="40"/>
     </row>
     <row r="15" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="21" t="s">
+      <c r="D15" s="32"/>
+      <c r="E15" s="41" t="s">
         <v>36</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="39">
         <v>43872</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="35"/>
       <c r="F16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="31"/>
+      <c r="G16" s="42"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="22"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="36"/>
       <c r="F17" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="40"/>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="25"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="32" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G18" s="39">
         <v>43875</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27" t="s">
+      <c r="A19" s="38"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="27"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="31"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="42"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="31"/>
+      <c r="G20" s="42"/>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="9" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="31"/>
+      <c r="G21" s="42"/>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="34"/>
       <c r="C22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="26"/>
+      <c r="D22" s="34"/>
       <c r="E22" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="30"/>
+      <c r="G22" s="40"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -1291,39 +1294,39 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="F29" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="G29" s="37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
     </row>
     <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="24" t="s">
         <v>49</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -1332,67 +1335,67 @@
       <c r="C31" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="25"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="12" t="s">
         <v>54</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="38">
+      <c r="G31" s="27">
         <v>43882</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="18"/>
       <c r="C32" s="15"/>
-      <c r="D32" s="27"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="15"/>
       <c r="F32" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="39"/>
+      <c r="G32" s="28"/>
     </row>
     <row r="33" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
-      <c r="B33" s="28" t="s">
+      <c r="A33" s="25"/>
+      <c r="B33" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="27"/>
-      <c r="E33" s="41" t="s">
+      <c r="D33" s="33"/>
+      <c r="E33" s="30" t="s">
         <v>56</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G33" s="39"/>
+      <c r="G33" s="28"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="42"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="31"/>
       <c r="F34" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G34" s="40"/>
+      <c r="G34" s="29"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="34"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="14" t="s">
         <v>59</v>
       </c>
@@ -1401,13 +1404,13 @@
       <c r="A36" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B36" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="34"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="14" t="s">
         <v>61</v>
       </c>
@@ -1438,7 +1441,7 @@
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="G38" s="2"/>
     </row>
@@ -1534,44 +1537,6 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G22"/>
-    <mergeCell ref="F29:F30"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="A15:A17"/>
@@ -1586,6 +1551,44 @@
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="D18:D22"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G22"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B33:B34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finish initial analytics features with timesheet and sales records
</commit_message>
<xml_diff>
--- a/documentation/Version History.xlsx
+++ b/documentation/Version History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siclait\Desktop\MiniMarketInventoryManagement\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DC9B94-BBAC-42F2-AC09-E964DE9EC4A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC9E5FC-2E39-46C4-932C-B44631F77376}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{F7D18C05-31F1-4F48-87A8-61387A74A440}"/>
   </bookViews>
@@ -210,15 +210,9 @@
     <t>v0.6.1</t>
   </si>
   <si>
-    <t>21 Fed</t>
-  </si>
-  <si>
     <t>v0.6.2</t>
   </si>
   <si>
-    <t>22 Fed</t>
-  </si>
-  <si>
     <t>Code Refactoring (Business Layer Namespaces)</t>
   </si>
   <si>
@@ -268,6 +262,12 @@
   </si>
   <si>
     <t>User Timesheet Bubble Chart</t>
+  </si>
+  <si>
+    <t>B6 = Twin Graphs Form Appear</t>
+  </si>
+  <si>
+    <t>User Sales Bar Graph</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -444,9 +444,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -456,9 +453,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -468,31 +462,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -504,34 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -544,6 +490,66 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,52 +866,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3F8C43-F028-4E57-9D96-908845B50375}">
   <dimension ref="A2:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="44"/>
+    <col min="1" max="1" width="11.42578125" style="26"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="6" max="6" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="39" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3"/>
@@ -916,7 +922,7 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -933,266 +939,266 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="31" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="36">
         <v>43856</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="29"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="27"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="38"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="22"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="36">
         <v>43859</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="26"/>
+      <c r="F9" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="24"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="24"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="29"/>
-      <c r="G10" s="27"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="38"/>
     </row>
     <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="31" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="36">
         <v>43862</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="13" t="s">
+      <c r="D12" s="32"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="26"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="23" t="s">
+      <c r="D13" s="32"/>
+      <c r="E13" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="26"/>
+      <c r="F13" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="37"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="29"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="27"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="38"/>
     </row>
     <row r="15" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="30" t="s">
+      <c r="D15" s="28"/>
+      <c r="E15" s="31" t="s">
         <v>36</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="36">
         <v>43872</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="13" t="s">
+      <c r="A16" s="30"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="26"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="29"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="33"/>
       <c r="F17" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="27"/>
+        <v>69</v>
+      </c>
+      <c r="G17" s="38"/>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="22"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="36">
         <v>43875</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23" t="s">
+      <c r="A19" s="30"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23" t="s">
+      <c r="D19" s="27"/>
+      <c r="E19" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="23"/>
-      <c r="G19" s="26"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="37"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="13" t="s">
+      <c r="A20" s="30"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="26"/>
+      <c r="G20" s="37"/>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="9" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="26"/>
+        <v>69</v>
+      </c>
+      <c r="G21" s="37"/>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="24"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="24"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" s="27"/>
+        <v>66</v>
+      </c>
+      <c r="G22" s="38"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1201,7 +1207,7 @@
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1210,7 +1216,7 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1219,7 +1225,7 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1227,227 +1233,235 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="36" t="s">
+      <c r="E27" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="36" t="s">
+      <c r="F27" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="36" t="s">
+      <c r="G27" s="34" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
     </row>
     <row r="29" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="30" t="s">
+      <c r="D29" s="28"/>
+      <c r="E29" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29" s="36">
         <v>43882</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="39"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="17" t="s">
+      <c r="A30" s="44"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="26"/>
+      <c r="G30" s="37"/>
     </row>
     <row r="31" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39"/>
-      <c r="B31" s="28" t="s">
+      <c r="A31" s="44"/>
+      <c r="B31" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="28" t="s">
+      <c r="D31" s="27"/>
+      <c r="E31" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G31" s="26"/>
+      <c r="G31" s="37"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G32" s="27"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="38"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="11" t="s">
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="46">
+        <v>43882</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="41" t="s">
+      <c r="B34" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="46">
+        <v>43883</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="28"/>
+      <c r="C35" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="15" t="s">
+      <c r="E35" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="2"/>
+      <c r="G35" s="36">
+        <v>43901</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
-      <c r="B36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="31" t="s">
+      <c r="A36" s="44"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G36" s="37"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="44"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G37" s="37"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="44"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G38" s="37"/>
+    </row>
+    <row r="39" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="44"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="32"/>
+      <c r="E39" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F39" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="G39" s="37"/>
+    </row>
+    <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="44"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="42"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="32" t="s">
+      <c r="F40" s="32"/>
+      <c r="G40" s="37"/>
+    </row>
+    <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="44"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2" t="s">
+      <c r="F41" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="42"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="15" t="s">
+      <c r="G41" s="37"/>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="45"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="F41" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="38"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="42"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1456,7 +1470,7 @@
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="43"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1465,7 +1479,7 @@
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="43"/>
+      <c r="A45" s="25"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1474,7 +1488,7 @@
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="43"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1483,7 +1497,7 @@
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="43"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1492,7 +1506,7 @@
       <c r="G47" s="1"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="43"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1501,35 +1515,21 @@
       <c r="G48" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G22"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
+  <mergeCells count="65">
+    <mergeCell ref="G35:G42"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="D35:D42"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="E29:E30"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="G6:G7"/>
@@ -1543,22 +1543,44 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G22"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="E19:E20"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B34:F34"/>
     <mergeCell ref="A29:A32"/>
-    <mergeCell ref="G29:G32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="E29:E30"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="E27:E28"/>
     <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="A35:A42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Create stored procedure to register unsuccessful log outs due to system crashes of unsuccessful log out protocols
</commit_message>
<xml_diff>
--- a/documentation/Version History.xlsx
+++ b/documentation/Version History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siclait\Desktop\MiniMarketInventoryManagement\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85F8DFB-448C-4454-907C-A14E16370AB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AEF36C-6A54-4918-B079-EC510F92E01C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{F7D18C05-31F1-4F48-87A8-61387A74A440}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="85">
   <si>
     <t xml:space="preserve">Mechanics </t>
   </si>
@@ -189,9 +189,6 @@
     <t>Structurized Data Management</t>
   </si>
   <si>
-    <t>B3 = FIXED</t>
-  </si>
-  <si>
     <t>Transaction Returns and Voiding</t>
   </si>
   <si>
@@ -234,9 +231,6 @@
     <t>B4 = Ignored Units of Measuments</t>
   </si>
   <si>
-    <t>B4 = FIXED</t>
-  </si>
-  <si>
     <t>B2 = Child Remains Opened</t>
   </si>
   <si>
@@ -274,13 +268,31 @@
   </si>
   <si>
     <t>B2 = FIXED HERE</t>
+  </si>
+  <si>
+    <t>v0.7.1</t>
+  </si>
+  <si>
+    <t>B5 = FIXED HERE</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B3(F)</t>
+  </si>
+  <si>
+    <t>B4(F)</t>
+  </si>
+  <si>
+    <t>B2(F)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +308,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="double"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -418,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -502,14 +522,44 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -517,46 +567,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -875,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3F8C43-F028-4E57-9D96-908845B50375}">
   <dimension ref="A2:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,36 +917,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="47" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -948,263 +977,263 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="41" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="44">
         <v>43856</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="46"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="35"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="44">
         <v>43859</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="36"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="36"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="G9" s="30"/>
+      <c r="F9" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="45"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="37"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="37"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="31"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="46"/>
     </row>
     <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="41" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="29" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="44">
         <v>43862</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="32"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="36"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="30"/>
+      <c r="G12" s="45"/>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="32"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="36" t="s">
+      <c r="D13" s="42"/>
+      <c r="E13" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="G13" s="30"/>
+      <c r="F13" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="45"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="33"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="43"/>
       <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="31"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="46"/>
     </row>
     <row r="15" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="34" t="s">
+      <c r="D15" s="29"/>
+      <c r="E15" s="41" t="s">
         <v>36</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="44">
         <v>43872</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="32"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="30"/>
+      <c r="G16" s="45"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="33"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="31"/>
+        <v>67</v>
+      </c>
+      <c r="G17" s="46"/>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="35"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G18" s="44">
         <v>43875</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36" t="s">
+      <c r="A19" s="40"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36" t="s">
+      <c r="D19" s="30"/>
+      <c r="E19" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="45"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="30"/>
+      <c r="G20" s="45"/>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="9" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" s="30"/>
+        <v>67</v>
+      </c>
+      <c r="G21" s="45"/>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
-      <c r="B22" s="37"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="37"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="31"/>
+        <v>65</v>
+      </c>
+      <c r="G22" s="46"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
@@ -1242,240 +1271,244 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="40" t="s">
+      <c r="E27" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="40" t="s">
+      <c r="F27" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="40" t="s">
+      <c r="G27" s="38" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
     </row>
     <row r="29" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="29"/>
+      <c r="E29" s="41" t="s">
         <v>53</v>
-      </c>
-      <c r="D29" s="35"/>
-      <c r="E29" s="34" t="s">
-        <v>54</v>
       </c>
       <c r="F29" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="29">
+      <c r="G29" s="44">
         <v>43882</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="32"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="42"/>
       <c r="F30" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="30"/>
+      <c r="G30" s="45"/>
     </row>
     <row r="31" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="46"/>
-      <c r="B31" s="32" t="s">
+      <c r="A31" s="33"/>
+      <c r="B31" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="30"/>
+      <c r="E31" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="36"/>
-      <c r="E31" s="32" t="s">
-        <v>56</v>
-      </c>
       <c r="F31" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="30"/>
+        <v>76</v>
+      </c>
+      <c r="G31" s="45"/>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="33"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="43"/>
       <c r="F32" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="G32" s="31"/>
+        <v>77</v>
+      </c>
+      <c r="G32" s="46"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="44"/>
+      <c r="B33" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="37"/>
       <c r="G33" s="28">
         <v>43882</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="44"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="37"/>
       <c r="G34" s="28">
         <v>43883</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="29"/>
+      <c r="C35" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="34" t="s">
+      <c r="E35" s="20" t="s">
         <v>63</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>64</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="29">
+      <c r="G35" s="44">
         <v>43901</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32" t="s">
+      <c r="A36" s="33"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="45"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="33"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="G37" s="45"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="33"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" s="45"/>
+    </row>
+    <row r="39" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="33"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="42"/>
+      <c r="E39" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39" s="45"/>
+    </row>
+    <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="33"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="F36" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="G36" s="30"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G37" s="30"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="G38" s="30"/>
-    </row>
-    <row r="39" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="46"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="32" t="s">
+      <c r="F40" s="42"/>
+      <c r="G40" s="45"/>
+    </row>
+    <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="33"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D39" s="32"/>
-      <c r="E39" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F39" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="G39" s="30"/>
-    </row>
-    <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="46"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="17" t="s">
+      <c r="F41" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="F40" s="32"/>
-      <c r="G40" s="30"/>
-    </row>
-    <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="46"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="18" t="s">
+      <c r="G41" s="45"/>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="34"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="F41" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="G41" s="30"/>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="47"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="F42" s="33"/>
-      <c r="G42" s="31"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="46"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
+      <c r="A43" s="23" t="s">
+        <v>79</v>
+      </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1484,7 +1517,9 @@
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+      <c r="F44" s="50" t="s">
+        <v>84</v>
+      </c>
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1493,7 +1528,9 @@
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+      <c r="F45" s="49" t="s">
+        <v>82</v>
+      </c>
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1502,16 +1539,20 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="F46" s="49" t="s">
+        <v>83</v>
+      </c>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="24"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="F47" s="48" t="s">
+        <v>80</v>
+      </c>
       <c r="G47" s="1"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1520,48 +1561,28 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="F48" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="G48" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G22"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G35:G42"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="D35:D42"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="E29:E30"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="G6:G7"/>
@@ -1575,21 +1596,43 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="G29:G32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="G35:G42"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="D35:D42"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G22"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improve timesheet bubble grpah analytics accuracy with decimal convertion of log in timestamp
</commit_message>
<xml_diff>
--- a/documentation/Version History.xlsx
+++ b/documentation/Version History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siclait\Desktop\MiniMarketInventoryManagement\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AEF36C-6A54-4918-B079-EC510F92E01C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FA207E-6C33-496A-8C9A-014B0C7E7A46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{F7D18C05-31F1-4F48-87A8-61387A74A440}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
   <si>
     <t xml:space="preserve">Mechanics </t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>B2(F)</t>
+  </si>
+  <si>
+    <t>Protocol 66</t>
+  </si>
+  <si>
+    <t>Improve Accuracy of Timesheet Graph</t>
   </si>
 </sst>
 </file>
@@ -438,12 +444,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -508,9 +511,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -525,67 +525,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -904,685 +907,719 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3F8C43-F028-4E57-9D96-908845B50375}">
   <dimension ref="A2:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43:B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="25"/>
+    <col min="1" max="1" width="11.42578125" style="23"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="6" max="6" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="E2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="47" t="s">
+      <c r="F2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="40" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="10">
+      <c r="F5" s="2"/>
+      <c r="G5" s="9">
         <v>43853</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="44">
+      <c r="G6" s="31">
         <v>43856</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="5" t="s">
+      <c r="A7" s="41"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="46"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="37"/>
+      <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="37"/>
+      <c r="E8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="44">
+      <c r="G8" s="31">
         <v>43859</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="6" t="s">
+      <c r="A9" s="41"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="38"/>
+      <c r="E9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="45"/>
+      <c r="G9" s="32"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="5" t="s">
+      <c r="A10" s="41"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="8" t="s">
+      <c r="D10" s="39"/>
+      <c r="E10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="46"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="44">
+      <c r="G11" s="31">
         <v>43862</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="6" t="s">
+      <c r="A12" s="41"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="12" t="s">
+      <c r="D12" s="34"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="45"/>
+      <c r="G12" s="32"/>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="6" t="s">
+      <c r="A13" s="41"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="30" t="s">
+      <c r="D13" s="34"/>
+      <c r="E13" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="45"/>
+      <c r="G13" s="32"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="5" t="s">
+      <c r="A14" s="41"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="46"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="41" t="s">
+      <c r="D15" s="37"/>
+      <c r="E15" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="44">
+      <c r="G15" s="31">
         <v>43872</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="12" t="s">
+      <c r="A16" s="41"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="45"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="8" t="s">
+      <c r="A17" s="41"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="46"/>
+      <c r="G17" s="33"/>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="37"/>
+      <c r="C18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="44">
+      <c r="G18" s="31">
         <v>43875</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30" t="s">
+      <c r="A19" s="41"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30" t="s">
+      <c r="D19" s="38"/>
+      <c r="E19" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="30"/>
-      <c r="G19" s="45"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="12" t="s">
+      <c r="A20" s="41"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="45"/>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="9" t="s">
+      <c r="A21" s="41"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="45"/>
+      <c r="G21" s="32"/>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="5" t="s">
+      <c r="A22" s="41"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="31"/>
-      <c r="E22" s="5" t="s">
+      <c r="D22" s="39"/>
+      <c r="E22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G22" s="46"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="38" t="s">
+      <c r="F27" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="38" t="s">
+      <c r="G27" s="42" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="39"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
     </row>
     <row r="29" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="29"/>
-      <c r="E29" s="41" t="s">
+      <c r="D29" s="37"/>
+      <c r="E29" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="44">
+      <c r="G29" s="31">
         <v>43882</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="15" t="s">
+      <c r="A30" s="45"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="45"/>
+      <c r="G30" s="32"/>
     </row>
     <row r="31" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
-      <c r="B31" s="42" t="s">
+      <c r="A31" s="45"/>
+      <c r="B31" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="42" t="s">
+      <c r="C31" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="30"/>
-      <c r="E31" s="42" t="s">
+      <c r="D31" s="38"/>
+      <c r="E31" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="G31" s="45"/>
+      <c r="G31" s="32"/>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="27" t="s">
+      <c r="A32" s="46"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="G32" s="46"/>
+      <c r="G32" s="33"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="28">
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="26">
         <v>43882</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="28">
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="26">
         <v>43883</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="41" t="s">
+      <c r="B35" s="37"/>
+      <c r="C35" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="41" t="s">
+      <c r="D35" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="44">
+      <c r="G35" s="31">
         <v>43901</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42" t="s">
+      <c r="A36" s="45"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="26" t="s">
+      <c r="F36" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="G36" s="45"/>
+      <c r="G36" s="32"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="49" t="s">
+      <c r="A37" s="45"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="G37" s="45"/>
+      <c r="G37" s="32"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="49" t="s">
+      <c r="A38" s="45"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="G38" s="45"/>
+      <c r="G38" s="32"/>
     </row>
     <row r="39" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="42" t="s">
+      <c r="A39" s="45"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="42"/>
-      <c r="E39" s="18" t="s">
+      <c r="D39" s="34"/>
+      <c r="E39" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="F39" s="42" t="s">
+      <c r="F39" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="G39" s="45"/>
+      <c r="G39" s="32"/>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="17" t="s">
+      <c r="A40" s="45"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F40" s="42"/>
-      <c r="G40" s="45"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="32"/>
     </row>
     <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="18" t="s">
+      <c r="A41" s="45"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="F41" s="42" t="s">
+      <c r="F41" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="G41" s="45"/>
+      <c r="G41" s="32"/>
     </row>
     <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="19" t="s">
+      <c r="A42" s="46"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F42" s="43"/>
-      <c r="G42" s="46"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
+      <c r="F42" s="35"/>
+      <c r="G42" s="33"/>
+    </row>
+    <row r="43" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2" t="s">
+      <c r="B43" s="37"/>
+      <c r="C43" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43" s="37"/>
+      <c r="F43" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G43" s="2"/>
+      <c r="G43" s="31">
+        <v>43901</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="50" t="s">
+      <c r="A44" s="45"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="G44" s="1"/>
+      <c r="G44" s="32"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="49" t="s">
+      <c r="A45" s="45"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="G45" s="1"/>
+      <c r="G45" s="32"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="49" t="s">
+      <c r="A46" s="45"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="G46" s="1"/>
+      <c r="G46" s="32"/>
     </row>
     <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="24"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="48" t="s">
+      <c r="A47" s="45"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="G47" s="1"/>
+      <c r="G47" s="32"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="24"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="2" t="s">
+      <c r="A48" s="46"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="G48" s="1"/>
+      <c r="G48" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="65">
-    <mergeCell ref="G35:G42"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="D35:D42"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="G29:G32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="E29:E30"/>
+  <mergeCells count="71">
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="G43:G48"/>
+    <mergeCell ref="E43:E48"/>
+    <mergeCell ref="D43:D48"/>
+    <mergeCell ref="C43:C48"/>
+    <mergeCell ref="B43:B48"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G22"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="G6:G7"/>
@@ -1596,43 +1633,21 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G22"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="G35:G42"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="D35:D42"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="E36:E38"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
BUG FIX: working 72 hour options in user timesheet bubble chart
</commit_message>
<xml_diff>
--- a/documentation/Version History.xlsx
+++ b/documentation/Version History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siclait\Desktop\MiniMarketInventoryManagement\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FA207E-6C33-496A-8C9A-014B0C7E7A46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DBA67E-A294-4320-84F4-A1D66D41C677}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{F7D18C05-31F1-4F48-87A8-61387A74A440}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="92">
   <si>
     <t xml:space="preserve">Mechanics </t>
   </si>
@@ -261,21 +261,9 @@
     <t>User Sales Bar Graph</t>
   </si>
   <si>
-    <t>B3 = FIXED HERE</t>
-  </si>
-  <si>
-    <t>B4 = FIXED HERE</t>
-  </si>
-  <si>
-    <t>B2 = FIXED HERE</t>
-  </si>
-  <si>
     <t>v0.7.1</t>
   </si>
   <si>
-    <t>B5 = FIXED HERE</t>
-  </si>
-  <si>
     <t>B6</t>
   </si>
   <si>
@@ -292,6 +280,33 @@
   </si>
   <si>
     <t>Improve Accuracy of Timesheet Graph</t>
+  </si>
+  <si>
+    <t>B7 = Faulty 72 Hour Option</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>v0.8.0</t>
+  </si>
+  <si>
+    <t>B5(F)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B7 = FIXED </t>
+  </si>
+  <si>
+    <t>B3 = FIXED</t>
+  </si>
+  <si>
+    <t>B4 = FIXED</t>
+  </si>
+  <si>
+    <t>B2 = FIXED</t>
+  </si>
+  <si>
+    <t>B5 = FIXED</t>
   </si>
 </sst>
 </file>
@@ -444,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -474,24 +489,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -501,95 +522,82 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -905,54 +913,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3F8C43-F028-4E57-9D96-908845B50375}">
-  <dimension ref="A2:G48"/>
+  <dimension ref="A2:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43:B48"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="23"/>
+    <col min="1" max="1" width="11.42578125" style="44"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="46" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="43" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="24" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2"/>
@@ -963,7 +971,7 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="24" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -980,266 +988,266 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="34" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="28">
         <v>43856</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="35"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="30"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="37"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="28">
         <v>43859</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="38"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="38"/>
+      <c r="D9" s="32"/>
       <c r="E9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="29"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="39"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="35"/>
-      <c r="G10" s="33"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="30"/>
     </row>
     <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="34" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="28">
         <v>43862</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="34"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="11" t="s">
+      <c r="D12" s="35"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="29"/>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="34"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="38" t="s">
+      <c r="D13" s="35"/>
+      <c r="E13" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="32"/>
+      <c r="G13" s="29"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="35"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="33"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="30"/>
     </row>
     <row r="15" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="36" t="s">
+      <c r="D15" s="31"/>
+      <c r="E15" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="28">
         <v>43872</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="11" t="s">
+      <c r="A16" s="42"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="32"/>
+      <c r="G16" s="29"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="7" t="s">
+      <c r="A17" s="42"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="33"/>
+      <c r="G17" s="30"/>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="37"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="28">
         <v>43875</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38" t="s">
+      <c r="A19" s="42"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38" t="s">
+      <c r="D19" s="32"/>
+      <c r="E19" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="38"/>
-      <c r="G19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="29"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="11" t="s">
+      <c r="A20" s="42"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="32"/>
+      <c r="G20" s="29"/>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
       <c r="E21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="32"/>
+      <c r="G21" s="29"/>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="39"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="39"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="G22" s="33"/>
+      <c r="G22" s="30"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1248,7 +1256,7 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1257,7 +1265,7 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1266,7 +1274,7 @@
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1274,352 +1282,413 @@
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="42" t="s">
+      <c r="E27" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="42" t="s">
+      <c r="F27" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="42" t="s">
+      <c r="G27" s="40" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
     </row>
     <row r="29" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="37"/>
-      <c r="E29" s="36" t="s">
+      <c r="D29" s="31"/>
+      <c r="E29" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="31">
+      <c r="G29" s="28">
         <v>43882</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="45"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="14" t="s">
+      <c r="A30" s="26"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="32"/>
+      <c r="G30" s="29"/>
     </row>
     <row r="31" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="45"/>
-      <c r="B31" s="34" t="s">
+      <c r="A31" s="26"/>
+      <c r="B31" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="38"/>
-      <c r="E31" s="34" t="s">
+      <c r="D31" s="32"/>
+      <c r="E31" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="29"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="27"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G32" s="30"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="17">
+        <v>43882</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="17">
+        <v>43883</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="28">
+        <v>43901</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G36" s="29"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="26"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G37" s="29"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="26"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G38" s="29"/>
+    </row>
+    <row r="39" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="26"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="35"/>
+      <c r="E39" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39" s="29"/>
+    </row>
+    <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="26"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="35"/>
+      <c r="G40" s="29"/>
+    </row>
+    <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="26"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G41" s="29"/>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="27"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G42" s="30"/>
+    </row>
+    <row r="43" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="G31" s="32"/>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="46"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="25" t="s">
+      <c r="B43" s="31"/>
+      <c r="C43" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" s="31"/>
+      <c r="F43" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="28">
+        <v>43901</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="26"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G44" s="29"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="26"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45" s="29"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="26"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46" s="29"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="26"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="G47" s="29"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="26"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="G32" s="33"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="26">
-        <v>43882</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="26">
-        <v>43883</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="37"/>
-      <c r="C35" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="F35" s="15" t="s">
+      <c r="G48" s="29"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="27"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="G49" s="30"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="F57" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="G57" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="41"/>
+      <c r="B58" s="41"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="41"/>
+      <c r="E58" s="41"/>
+      <c r="F58" s="41"/>
+      <c r="G58" s="41"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="F59" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="31">
-        <v>43901</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="45"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="F36" s="24" t="s">
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F60" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F61" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="G36" s="32"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="45"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="G37" s="32"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="45"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="G38" s="32"/>
-    </row>
-    <row r="39" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="45"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="34"/>
-      <c r="E39" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F39" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="G39" s="32"/>
-    </row>
-    <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="45"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F40" s="34"/>
-      <c r="G40" s="32"/>
-    </row>
-    <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="45"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F41" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="G41" s="32"/>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="46"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F42" s="35"/>
-      <c r="G42" s="33"/>
-    </row>
-    <row r="43" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="44" t="s">
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F62" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="37"/>
-      <c r="C43" s="36" t="s">
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F63" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="D43" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="E43" s="37"/>
-      <c r="F43" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G43" s="31">
-        <v>43901</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="45"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="G44" s="32"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="45"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="G45" s="32"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="45"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="G46" s="32"/>
-    </row>
-    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="45"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="G47" s="32"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="46"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="G48" s="33"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F64" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F65" s="23" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="71">
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="G43:G48"/>
-    <mergeCell ref="E43:E48"/>
-    <mergeCell ref="D43:D48"/>
-    <mergeCell ref="C43:C48"/>
-    <mergeCell ref="B43:B48"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G22"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
+  <mergeCells count="77">
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="G35:G42"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="D35:D42"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="E29:E30"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="G6:G7"/>
@@ -1633,21 +1702,49 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="G29:G32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="G35:G42"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="D35:D42"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G22"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A43:A49"/>
+    <mergeCell ref="G43:G49"/>
+    <mergeCell ref="E43:E49"/>
+    <mergeCell ref="D43:D49"/>
+    <mergeCell ref="C43:C49"/>
+    <mergeCell ref="B43:B49"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>